<commit_message>
Upgraded Fighter skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Done/1_Fighter/Documentation/FighterSkills.xlsx
+++ b/GameDesign/Class/Done/1_Fighter/Documentation/FighterSkills.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="81">
   <si>
     <t xml:space="preserve">Fighter Meditation </t>
   </si>
@@ -66,9 +66,6 @@
     <t>Fighter Aura</t>
   </si>
   <si>
-    <t>Unbuff ''Focus'' effect if a character hit another target.</t>
-  </si>
-  <si>
     <t>Effect name: ''Focus''.</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>[[Number of turns between two casts: 4  ]]</t>
   </si>
   <si>
-    <t>The cell must no be occupied.</t>
-  </si>
-  <si>
     <t>Iron Punch</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>[[Reduce target resistance by 20%]] (2 turns)</t>
   </si>
   <si>
-    <t>Must target an enemy.</t>
-  </si>
-  <si>
     <t>Ki Blast</t>
   </si>
   <si>
@@ -246,43 +237,40 @@
     <t>[[Reduce target resistance by 20%]] (1 turn) (50%)</t>
   </si>
   <si>
-    <t>If is an enemy, [[Damage:  27-30 earth ]]</t>
-  </si>
-  <si>
-    <t>Move opposite direction from target.</t>
-  </si>
-  <si>
-    <t>Increases the target's HP and resistances.</t>
-  </si>
-  <si>
-    <t>Increases the target's AP and power.</t>
-  </si>
-  <si>
-    <t>Reduces the enemy resistance. The caster and his allies must not dealt damages to another enemies otherwise that effect is cancelled.</t>
-  </si>
-  <si>
     <t>[[Damage:  (20*Precision lvl) air ]]</t>
   </si>
   <si>
-    <t>Inflicts Air-type damage. The damage dealt keep increasing if chaining this skill on the target.</t>
-  </si>
-  <si>
-    <t>Inflicts Earth-type damage. Move the caster in front of the target and increase the next Liquid Kick damage.</t>
-  </si>
-  <si>
-    <t>Inflicts Earth-type damage. Move the caster in the opposite direction and increase the next Iron Punch damage.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teleports at the targeted cell </t>
-  </si>
-  <si>
-    <t>Inflicts Earth-type damage and reduces the target power.</t>
-  </si>
-  <si>
-    <t>Inflicts Light-type damage and push the target. The push is stronger on target whit Focus effect.</t>
-  </si>
-  <si>
-    <t>Inflicts Water-type damage and reduces the target resistances. Also have a chance to dealt more damage and reduces more resistances.</t>
+    <t xml:space="preserve">Increases the target's HP and resistances.                              Remove the Fighter Aura effect if the target has it.                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increases the target's AP and power.                                       Remove the Fighter Meditation effect if the target has it.   </t>
+  </si>
+  <si>
+    <t>Reduces an enemy resistance.                                                         The caster and his allies must not dealt damages to another enemies otherwise that effect is cancelled.</t>
+  </si>
+  <si>
+    <t>Inflicts Air-type damage.                                                                   The damage dealt keep increasing if the skill is chained on the target.                                                                                                The damage increase faster if the target is under Focus effect.</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage to enemies.                                                            Move the caster in front of the target.                                      Increases the next Liquid Kick damage.</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage.                                                              Can only be used on enemies.                                                        Move the caster in the opposite direction.                               Increase the next Iron Punch damage.</t>
+  </si>
+  <si>
+    <t>Move in the opposite direction from target by 1 cell.</t>
+  </si>
+  <si>
+    <t>Teleports onto the targeted empty cell.</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage.                                                       Reduces the target power.</t>
+  </si>
+  <si>
+    <t>Inflicts Light-type damage.                                                             Push the target.                                                                                 The push is stronger on target whit Focus effect.</t>
+  </si>
+  <si>
+    <t>Inflicts Water-type damage.                                                      Reduces the target resistances.                                                      Chance to dealt more damage and reduces more resistances.</t>
   </si>
 </sst>
 </file>
@@ -322,7 +310,7 @@
       <family val="5"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,14 +335,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -397,11 +379,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -413,9 +410,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -425,8 +419,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -436,6 +428,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,10 +780,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="13" t="s">
-        <v>74</v>
+      <c r="C5" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -796,121 +794,121 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="6"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="6" t="s">
-        <v>47</v>
+      <c r="C17" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="6" t="s">
-        <v>48</v>
+      <c r="C18" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="16" t="s">
+        <v>46</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="1"/>
+      <c r="C23" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="9" t="s">
-        <v>9</v>
+      <c r="C25" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="10"/>
+      <c r="D26" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -943,7 +941,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -954,8 +952,8 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="14" t="s">
-        <v>84</v>
+      <c r="C5" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -966,63 +964,63 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="6" t="s">
-        <v>43</v>
+      <c r="C7" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
-        <v>34</v>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="6"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="7" t="s">
-        <v>28</v>
+      <c r="C12" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>64</v>
+      <c r="C14" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="6"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="6" t="s">
-        <v>62</v>
+      <c r="C16" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1033,29 +1031,29 @@
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="6" t="s">
-        <v>63</v>
+      <c r="C18" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="6" t="s">
-        <v>70</v>
+      <c r="C19" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="11" t="s">
-        <v>65</v>
+      <c r="C20" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="12" t="s">
-        <v>71</v>
+      <c r="C21" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1072,7 +1070,7 @@
     </row>
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="1"/>
@@ -1084,15 +1082,15 @@
     </row>
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="9" t="s">
-        <v>69</v>
+      <c r="C27" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="10"/>
+      <c r="D28" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1134,10 +1132,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="5" t="s">
-        <v>75</v>
+      <c r="C5" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1148,121 +1146,121 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="6"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="6" t="s">
-        <v>49</v>
+      <c r="C17" s="15" t="s">
+        <v>10</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="6" t="s">
-        <v>50</v>
+      <c r="C18" s="16" t="s">
+        <v>47</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="1"/>
+      <c r="C23" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="9" t="s">
-        <v>10</v>
+      <c r="C25" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="10"/>
+      <c r="D26" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1271,6 +1269,547 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D26"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="1"/>
+      <c r="C23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D27"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="1"/>
+      <c r="C19" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B24" s="1"/>
+      <c r="C24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B26" s="1"/>
+      <c r="C26" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D30"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1"/>
+      <c r="C21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B22" s="1"/>
+      <c r="C22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B27" s="1"/>
+      <c r="C27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B29" s="1"/>
+      <c r="C29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D28"/>
   <sheetViews>
@@ -1295,7 +1834,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1304,10 +1843,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="15" t="s">
-        <v>76</v>
+      <c r="C5" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1318,71 +1857,69 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="6" t="s">
-        <v>18</v>
+      <c r="C7" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
-        <v>17</v>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="6" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>14</v>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="7" t="s">
-        <v>5</v>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="1"/>
@@ -1394,575 +1931,22 @@
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B23" s="1"/>
-      <c r="C23" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B26" s="1"/>
-      <c r="C26" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B27" s="1"/>
-      <c r="C27" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D27"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="1"/>
-      <c r="C19" s="12" t="s">
-        <v>57</v>
+      <c r="C19" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B24" s="1"/>
-      <c r="C24" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B26" s="1"/>
-      <c r="C26" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D30"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B23" s="1"/>
-      <c r="C23" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B27" s="1"/>
-      <c r="C27" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B29" s="1"/>
-      <c r="C29" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D29"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="6" t="s">
-        <v>33</v>
+      <c r="C21" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1979,7 +1963,7 @@
     </row>
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="1"/>
@@ -1991,22 +1975,15 @@
     </row>
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="9" t="s">
-        <v>32</v>
+      <c r="C27" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="C28" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="10"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2039,7 +2016,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2051,7 +2028,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2062,71 +2039,71 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
-        <v>37</v>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="6" t="s">
-        <v>30</v>
+      <c r="C9" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="6"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="6" t="s">
-        <v>38</v>
+      <c r="C11" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="6" t="s">
-        <v>39</v>
+      <c r="C12" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="6" t="s">
-        <v>29</v>
+      <c r="C13" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="6" t="s">
-        <v>40</v>
+      <c r="C15" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="1"/>
@@ -2138,8 +2115,8 @@
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="6" t="s">
-        <v>68</v>
+      <c r="C19" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -2156,7 +2133,7 @@
     </row>
     <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="1"/>
@@ -2168,15 +2145,13 @@
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="9" t="s">
-        <v>41</v>
-      </c>
+      <c r="C25" s="8"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="10"/>
+      <c r="D26" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2209,7 +2184,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2218,10 +2193,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="14" t="s">
-        <v>82</v>
+      <c r="C5" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2232,69 +2207,69 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="6" t="s">
-        <v>43</v>
+      <c r="C7" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
-        <v>34</v>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="6"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="7" t="s">
-        <v>28</v>
+      <c r="C12" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>27</v>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="6" t="s">
-        <v>20</v>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="1"/>
@@ -2306,15 +2281,15 @@
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="6" t="s">
-        <v>44</v>
+      <c r="C19" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="6" t="s">
-        <v>58</v>
+      <c r="C20" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2331,7 +2306,7 @@
     </row>
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="1"/>
@@ -2343,15 +2318,15 @@
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="9" t="s">
-        <v>45</v>
+      <c r="C26" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="10"/>
+      <c r="D27" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2384,7 +2359,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2393,10 +2368,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="14" t="s">
-        <v>83</v>
+      <c r="C5" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2407,64 +2382,64 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="6" t="s">
-        <v>43</v>
+      <c r="C7" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
-        <v>60</v>
+      <c r="C8" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="6" t="s">
-        <v>38</v>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="6" t="s">
-        <v>16</v>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="6" t="s">
-        <v>29</v>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>54</v>
+      <c r="C14" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="6"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="1"/>
@@ -2476,22 +2451,22 @@
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="6" t="s">
-        <v>55</v>
+      <c r="C18" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="6" t="s">
-        <v>59</v>
+      <c r="C19" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="6" t="s">
-        <v>56</v>
+      <c r="C20" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2508,7 +2483,7 @@
     </row>
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="1"/>
@@ -2520,13 +2495,13 @@
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="9"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="10"/>
+      <c r="D27" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>